<commit_message>
Add examples for past and present job and immunization
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-eicr-anon-composition.xlsx
+++ b/output/StructureDefinition-eicr-anon-composition.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-13T06:51:52+10:00</t>
+    <t>2024-06-13T11:16:16+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -3183,7 +3183,7 @@
     <t>sliceODHPastOrPresentJob</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/odh/StructureDefinition/odh-PastOrPresentJob)
+    <t xml:space="preserve">Reference(http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-past-or-present-job)
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Added RR examples Update Organization processing constraints Renamed profiles to be more consistent
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-eicr-anon-composition.xlsx
+++ b/output/StructureDefinition-eicr-anon-composition.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-13T11:16:16+10:00</t>
+    <t>2024-06-18T16:49:21+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -950,7 +950,7 @@
     <t>Composition.author</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-practitionerrole|http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-practitioner|http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-organization|Device)
+    <t xml:space="preserve">Reference(http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-practitionerrole|http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-practitioner|http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-org-tele-addr|Device)
 </t>
   </si>
   <si>
@@ -1162,7 +1162,7 @@
     <t>Composition.custodian</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-org-telecom)
+    <t xml:space="preserve">Reference(http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-org-tele)
 </t>
   </si>
   <si>
@@ -3296,13 +3296,13 @@
     <t>Country of nationality entry</t>
   </si>
   <si>
-    <t>Composition.section:sliceSocialHistorySection.entry:sliceCalculatedAge</t>
-  </si>
-  <si>
-    <t>sliceCalculatedAge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/caculated-age-observation)
+    <t>Composition.section:sliceSocialHistorySection.entry:sliceEICRAnonymizedCalculatedAge</t>
+  </si>
+  <si>
+    <t>sliceEICRAnonymizedCalculatedAge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-caculated-age)
 </t>
   </si>
   <si>
@@ -4122,7 +4122,7 @@
     <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="246.1875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="246.90625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Update to remove name, address, telecom anonymization constraints on Organization and Location (other than in the case of ODH Employer).
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-eicr-anon-composition.xlsx
+++ b/output/StructureDefinition-eicr-anon-composition.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-21T11:31:43+10:00</t>
+    <t>2024-06-25T09:09:40+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1162,11 +1162,11 @@
     <t>Composition.custodian</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-org-tele)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/ecr/StructureDefinition/us-ph-organization)
 </t>
   </si>
   <si>
-    <t>References the eICR Anonymized Organization - Telecom</t>
+    <t>Organization which maintains the composition</t>
   </si>
   <si>
     <t>Identifies the organization or group who is responsible for ongoing maintenance of and access to the composition/document information.</t>

</xml_diff>

<commit_message>
Change anonymized organization profile name to align with others Removed old anoymized organization profiles that are no longer needed
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-eicr-anon-composition.xlsx
+++ b/output/StructureDefinition-eicr-anon-composition.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-25T09:09:40+10:00</t>
+    <t>2024-06-26T05:55:02+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -950,7 +950,7 @@
     <t>Composition.author</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-practitionerrole|http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-practitioner|http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-org-tele-addr|Device)
+    <t xml:space="preserve">Reference(http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-practitionerrole|http://fhir.org/fhir/us/anonymized-eicr/StructureDefinition/eicr-anon-practitioner|http://hl7.org/fhir/us/ecr/StructureDefinition/us-ph-organization|Device)
 </t>
   </si>
   <si>
@@ -4122,7 +4122,7 @@
     <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="246.90625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="230.2890625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Updates to guidance in profiles, text descriptions of masked elements etc.
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-eicr-anon-composition.xlsx
+++ b/output/StructureDefinition-eicr-anon-composition.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-26T05:55:02+10:00</t>
+    <t>2024-06-26T06:31:28+10:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -954,7 +954,7 @@
 </t>
   </si>
   <si>
-    <t>References the eICR Anonymized PractitionerRole, eICR Anonymized Practitioner, eICR Anonymized Organization, or Device</t>
+    <t>References the eICR Anonymized PractitionerRole, eICR Anonymized Practitioner, US Public Health Organization, or Device</t>
   </si>
   <si>
     <t>It is possible to have multiple authors - especially in the case where the default author is the organization. For public health reporting this could contain the contact details for the Infection Control Professional (ICP) specific to the condition being reported on. If the main author of the document is not a person, it is recommended to have an additional person author contact who is specific for a disease for follow-up requirements. This person could be the ICP. Where a trigger occurs outside of an encounter the author will represent the Provider and Facility for reporting purposes.</t>

</xml_diff>